<commit_message>
21 de agosto de 2023 - Lap HP
Se actualiza nuevamente el repositorio del curso de Física 1 Plan Cuatrimestral
</commit_message>
<xml_diff>
--- a/Combinacion/Bitacora_Fisica_1_NRC_240_Tercer_Parcial.xlsx
+++ b/Combinacion/Bitacora_Fisica_1_NRC_240_Tercer_Parcial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Cuatrimestral\Fisica_1_BC\Combinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC144FF-670F-407D-AE59-990C4925739D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E31EDF-9FC2-4018-A8D0-C28720F6ECDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0F235AD7-D688-432D-9EC9-BBED3FA60CFC}"/>
   </bookViews>
@@ -752,17 +752,7 @@
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1145,12 +1135,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8813936B-0508-409C-AE08-B9AA328C068F}">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5400" ySplit="975" topLeftCell="I1" activePane="bottomRight"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:T1048576"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="7980" ySplit="1155" topLeftCell="R6" activePane="bottomRight"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,18 +1760,18 @@
         <v>9</v>
       </c>
       <c r="P10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="1">
         <v>10</v>
       </c>
       <c r="R10" s="2">
         <f t="shared" si="2"/>
-        <v>6.333333333333333</v>
+        <v>9</v>
       </c>
       <c r="S10" s="2">
         <f t="shared" si="4"/>
-        <v>8.0016666666666669</v>
+        <v>8.8016666666666659</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2090,18 +2080,18 @@
         <v>9</v>
       </c>
       <c r="P15" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="1">
         <v>10</v>
       </c>
       <c r="R15" s="2">
         <f t="shared" si="2"/>
-        <v>6.333333333333333</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="S15" s="2">
         <f t="shared" si="4"/>
-        <v>8.0629166666666663</v>
+        <v>8.9629166666666666</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2221,15 +2211,15 @@
         <v>9</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R17" s="2">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S17" s="2">
         <f t="shared" si="4"/>
-        <v>8.2399999999999984</v>
+        <v>9.1399999999999988</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -2706,14 +2696,14 @@
         <v>0</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1">
         <v>3</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="1"/>
@@ -2727,21 +2717,21 @@
         <v>9.0166666666666657</v>
       </c>
       <c r="O25" s="2">
-        <v>9</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="P25" s="1">
-        <v>9</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="Q25" s="1">
         <v>10</v>
       </c>
       <c r="R25" s="2">
         <f t="shared" si="2"/>
-        <v>9.3333333333333339</v>
+        <v>9.4666666666666668</v>
       </c>
       <c r="S25" s="2">
         <f t="shared" si="4"/>
-        <v>9.1116666666666664</v>
+        <v>9.1516666666666655</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -3242,18 +3232,18 @@
         <v>9</v>
       </c>
       <c r="P33" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q33" s="1">
         <v>10</v>
       </c>
       <c r="R33" s="2">
         <f t="shared" si="2"/>
-        <v>6.333333333333333</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="S33" s="2">
         <f t="shared" si="4"/>
-        <v>7.336666666666666</v>
+        <v>8.2366666666666664</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -3437,15 +3427,15 @@
         <v>9</v>
       </c>
       <c r="Q36" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R36" s="2">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S36" s="2">
         <f t="shared" si="4"/>
-        <v>7.6449999999999996</v>
+        <v>8.5449999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -3721,10 +3711,10 @@
         <v>139</v>
       </c>
       <c r="F41" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G41" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H41" s="1">
         <v>1</v>
@@ -3737,18 +3727,18 @@
       </c>
       <c r="K41" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L41" s="2">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.5</v>
       </c>
       <c r="M41" s="2">
         <v>7.3666666666666663</v>
       </c>
       <c r="N41" s="2">
         <f t="shared" si="3"/>
-        <v>3.9333333333333331</v>
+        <v>6.9333333333333336</v>
       </c>
       <c r="O41" s="2">
         <v>9</v>
@@ -3765,7 +3755,7 @@
       </c>
       <c r="S41" s="2">
         <f t="shared" si="4"/>
-        <v>4.6533333333333324</v>
+        <v>6.7533333333333339</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3913,10 +3903,10 @@
         <v>147</v>
       </c>
       <c r="F44" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G44" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
@@ -3925,22 +3915,22 @@
         <v>1</v>
       </c>
       <c r="J44" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K44" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="L44" s="2">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>7</v>
       </c>
       <c r="M44" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N44" s="2">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>5.5</v>
       </c>
       <c r="O44" s="2">
         <v>0</v>
@@ -3957,7 +3947,7 @@
       </c>
       <c r="S44" s="2">
         <f t="shared" si="4"/>
-        <v>0.17499999999999999</v>
+        <v>3.8499999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -4157,21 +4147,16 @@
     <sortCondition ref="B3:B47"/>
   </sortState>
   <conditionalFormatting sqref="F3:G47">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:N47">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R47">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
-      <formula>6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S47">
+  <conditionalFormatting sqref="R3:S47">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>6</formula>
     </cfRule>
@@ -12243,8 +12228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006EF051-549F-459E-8651-7D23499FAC6B}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12381,11 +12366,11 @@
         <v>5.9667178362573097</v>
       </c>
       <c r="L3" s="2">
-        <v>6.8116666666666656</v>
+        <v>7.7</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M45" si="2">SUM(F3:G3,L3)/3</f>
-        <v>5.6706067251461976</v>
+        <v>5.9667178362573097</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -12645,11 +12630,11 @@
         <v>6.9715350877192988</v>
       </c>
       <c r="L9" s="2">
-        <v>8.0016666666666669</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
-        <v>7.3054239766081865</v>
+        <v>7.5715350877192975</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -12865,11 +12850,11 @@
         <v>7.6261111111111104</v>
       </c>
       <c r="L14" s="2">
-        <v>8.0629166666666663</v>
+        <v>9</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="2"/>
-        <v>7.9804166666666658</v>
+        <v>8.2927777777777774</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12953,11 +12938,11 @@
         <v>7.1061111111111117</v>
       </c>
       <c r="L16" s="2">
-        <v>8.2399999999999984</v>
+        <v>9</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
-        <v>7.852777777777777</v>
+        <v>8.1061111111111117</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -12997,11 +12982,11 @@
         <v>6.7094444444444434</v>
       </c>
       <c r="L17" s="2">
-        <v>8.1783333333333328</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="2"/>
-        <v>7.1022222222222213</v>
+        <v>7.4761111111111118</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -13041,11 +13026,11 @@
         <v>6.0134210526315783</v>
       </c>
       <c r="L18" s="2">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="2"/>
-        <v>6.313421052631579</v>
+        <v>6.3800877192982455</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -13129,11 +13114,11 @@
         <v>6.0576608187134502</v>
       </c>
       <c r="L20" s="2">
-        <v>4.6783333333333328</v>
+        <v>7</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="2"/>
-        <v>5.6171052631578933</v>
+        <v>6.3909941520467832</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -13261,11 +13246,11 @@
         <v>7.2172222222222215</v>
       </c>
       <c r="L23" s="2">
-        <v>9.1116666666666664</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="M23" s="2">
         <f t="shared" si="2"/>
-        <v>7.9211111111111103</v>
+        <v>7.9505555555555558</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -13525,11 +13510,11 @@
         <v>7.3961111111111109</v>
       </c>
       <c r="L29" s="2">
-        <v>8.1783333333333328</v>
+        <v>8.4</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" si="2"/>
-        <v>8.1222222222222218</v>
+        <v>8.1961111111111098</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -13613,11 +13598,11 @@
         <v>5.9748245614035085</v>
       </c>
       <c r="L31" s="2">
-        <v>7.336666666666666</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" si="2"/>
-        <v>6.0537134502923964</v>
+        <v>6.3414912280701756</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -13745,11 +13730,11 @@
         <v>7.7061111111111105</v>
       </c>
       <c r="L34" s="2">
-        <v>7.6449999999999996</v>
+        <v>8.5</v>
       </c>
       <c r="M34" s="2">
         <f t="shared" si="2"/>
-        <v>7.9211111111111103</v>
+        <v>8.2061111111111114</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>